<commit_message>
progression data clean up
</commit_message>
<xml_diff>
--- a/Projet/GenDung/Assets/Extra/Balancing/GenDung_Balancing.xlsx
+++ b/Projet/GenDung/Assets/Extra/Balancing/GenDung_Balancing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity - Dungeon Project RP\Project\GenDung\Projet\GenDung\Assets\Extra\Balancing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB3AE6B-7661-4A73-B635-959F04944327}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23282BFA-A7FB-48A3-8FBD-00926B0424DE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{7D3B3BDF-DED2-4DA8-91A2-DF410998FF46}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7D3B3BDF-DED2-4DA8-91A2-DF410998FF46}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51957B96-EC4E-41AE-9449-2134AC46D0A9}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <f>L2*K2</f>
+        <f t="shared" ref="M2:M10" si="0">L2*K2</f>
         <v>0</v>
       </c>
       <c r="N2">
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" ref="H3:H10" si="0">G3*D3</f>
+        <f t="shared" ref="H3:H10" si="1">G3*D3</f>
         <v>20</v>
       </c>
       <c r="I3" s="6">
@@ -789,19 +789,19 @@
         <v>2</v>
       </c>
       <c r="M3">
-        <f>L3*K3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N10" si="1">M3+H3</f>
+        <f t="shared" ref="N3:N10" si="2">M3+H3</f>
         <v>26</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O10" si="2">IF(L3=0,N3,N3/(L3+1))</f>
+        <f t="shared" ref="O3:O10" si="3">IF(L3=0,N3,N3/(L3+1))</f>
         <v>8.6666666666666661</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P10" si="3">O3/E3</f>
+        <f t="shared" ref="P3:P10" si="4">O3/E3</f>
         <v>8.6666666666666661</v>
       </c>
     </row>
@@ -828,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I4" s="6">
@@ -846,19 +846,19 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <f>L4*K4</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="O4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
       <c r="P4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.25</v>
       </c>
       <c r="Q4" s="10">
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="I5" s="6">
@@ -911,19 +911,19 @@
         <v>1</v>
       </c>
       <c r="M5">
-        <f>L5*K5</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="P5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I6" s="6">
@@ -968,19 +968,19 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f>L6*K6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="O6">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
       <c r="P6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I7" s="6">
@@ -1025,19 +1025,19 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <f>L7*K7</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q7" s="10">
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I8" s="6">
@@ -1090,19 +1090,19 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <f>L8*K8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="O8">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
       <c r="P8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="I9" s="6">
@@ -1147,19 +1147,19 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f>L9*K9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="O9">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
       <c r="P9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="I10" s="6">
@@ -1204,19 +1204,19 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f>L10*K10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="O10">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
       <c r="P10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="Q10" s="10">
@@ -1460,11 +1460,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826E3668-8CED-439D-A07C-9AD6E97ABBC2}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1530,7 +1533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD5E520-1A24-417D-9D12-2AD7F38C1E20}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>